<commit_message>
making progress on excel
requirements.txt: updated requirements

Mixture_template.xlsx: fixed data error for density

main.py: using for debugging currently

read_excel.py: reading excel sheet well and getting things correctly but is very much hard coded and I dont like it, must refactor and add comments later

.gitignore: added cript_variables.py to ignore, so it is not pushed by accident
</commit_message>
<xml_diff>
--- a/assets/Mixture_template.xlsx
+++ b/assets/Mixture_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript SDK Learning\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F65B4C-2C4A-4E26-B546-9F871B8F4F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491A47E6-DE2E-45B8-8029-6342017F8D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,16 +485,16 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
     <col min="8" max="8" width="33.42578125" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
@@ -707,7 +707,7 @@
         <v>27</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -721,7 +721,7 @@
         <v>28</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="E13">
         <v>15</v>
@@ -784,9 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>